<commit_message>
Color to the game
</commit_message>
<xml_diff>
--- a/Reuniones_Coordinacion/I3_Gant_D1_Saul_Fernando_Raquel_Irene.xlsx
+++ b/Reuniones_Coordinacion/I3_Gant_D1_Saul_Fernando_Raquel_Irene.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\saul\Pprog_conversation\Reuniones_Coordinacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2951AE84-49FE-4709-882C-5DB837B4DC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBD74DF-C696-40C8-9316-2FC3898A5F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="2" xr2:uid="{05C49126-5558-4AD1-950B-328547F3A5DA}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" firstSheet="2" activeTab="3" xr2:uid="{05C49126-5558-4AD1-950B-328547F3A5DA}"/>
   </bookViews>
   <sheets>
     <sheet name="ASIGNACIÓN DE RECURSOS" sheetId="2" r:id="rId1"/>
     <sheet name="DIAGRAMA DE GANTT 18-3-2025" sheetId="1" r:id="rId2"/>
     <sheet name="DIAGRAMA DE GANTT 20-3-2025" sheetId="3" r:id="rId3"/>
+    <sheet name="DIAGRAMA DE GANTT 24-3-2025" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="84">
   <si>
     <t>CRONOGRAMA I2</t>
   </si>
@@ -804,7 +805,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -999,6 +1000,12 @@
     <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1062,12 +1069,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1475,115 +1485,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="105"/>
-      <c r="U1" s="105"/>
-      <c r="V1" s="105"/>
-      <c r="W1" s="105"/>
-      <c r="X1" s="105"/>
-      <c r="Y1" s="105"/>
-      <c r="Z1" s="105"/>
-      <c r="AA1" s="106"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="107"/>
+      <c r="T1" s="107"/>
+      <c r="U1" s="107"/>
+      <c r="V1" s="107"/>
+      <c r="W1" s="107"/>
+      <c r="X1" s="107"/>
+      <c r="Y1" s="107"/>
+      <c r="Z1" s="107"/>
+      <c r="AA1" s="108"/>
     </row>
     <row r="2" spans="1:28" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="102" t="s">
+      <c r="B2" s="101"/>
+      <c r="C2" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="107" t="s">
+      <c r="D2" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="111" t="s">
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="107"/>
-      <c r="S2" s="107"/>
-      <c r="T2" s="107"/>
-      <c r="U2" s="107"/>
-      <c r="V2" s="107"/>
-      <c r="W2" s="107"/>
-      <c r="X2" s="107"/>
-      <c r="Y2" s="107"/>
-      <c r="Z2" s="107"/>
-      <c r="AA2" s="112"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="109"/>
+      <c r="O2" s="109"/>
+      <c r="P2" s="109"/>
+      <c r="Q2" s="109"/>
+      <c r="R2" s="109"/>
+      <c r="S2" s="109"/>
+      <c r="T2" s="109"/>
+      <c r="U2" s="109"/>
+      <c r="V2" s="109"/>
+      <c r="W2" s="109"/>
+      <c r="X2" s="109"/>
+      <c r="Y2" s="109"/>
+      <c r="Z2" s="109"/>
+      <c r="AA2" s="114"/>
     </row>
     <row r="3" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="100"/>
-      <c r="B3" s="101"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="113" t="s">
+      <c r="A3" s="102"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="109"/>
-      <c r="J3" s="109"/>
-      <c r="K3" s="109"/>
-      <c r="L3" s="109"/>
-      <c r="M3" s="109" t="s">
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="109"/>
-      <c r="O3" s="109"/>
-      <c r="P3" s="109"/>
-      <c r="Q3" s="109"/>
-      <c r="R3" s="109" t="s">
+      <c r="N3" s="111"/>
+      <c r="O3" s="111"/>
+      <c r="P3" s="111"/>
+      <c r="Q3" s="111"/>
+      <c r="R3" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="109"/>
-      <c r="T3" s="109"/>
-      <c r="U3" s="109"/>
-      <c r="V3" s="109"/>
-      <c r="W3" s="109" t="s">
+      <c r="S3" s="111"/>
+      <c r="T3" s="111"/>
+      <c r="U3" s="111"/>
+      <c r="V3" s="111"/>
+      <c r="W3" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="109"/>
-      <c r="Y3" s="109"/>
-      <c r="Z3" s="109"/>
-      <c r="AA3" s="114"/>
+      <c r="X3" s="111"/>
+      <c r="Y3" s="111"/>
+      <c r="Z3" s="111"/>
+      <c r="AA3" s="116"/>
       <c r="AB3"/>
     </row>
     <row r="4" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="100"/>
-      <c r="B4" s="101"/>
-      <c r="C4" s="103"/>
+      <c r="A4" s="102"/>
+      <c r="B4" s="103"/>
+      <c r="C4" s="105"/>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
@@ -3592,8 +3602,8 @@
       <c r="AA51" s="73"/>
     </row>
     <row r="52" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="96"/>
-      <c r="B52" s="97"/>
+      <c r="A52" s="98"/>
+      <c r="B52" s="99"/>
       <c r="C52" s="74" t="s">
         <v>82</v>
       </c>
@@ -3613,26 +3623,26 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H52" s="94"/>
-      <c r="I52" s="94"/>
-      <c r="J52" s="94"/>
-      <c r="K52" s="94"/>
-      <c r="L52" s="94"/>
-      <c r="M52" s="94"/>
-      <c r="N52" s="94"/>
-      <c r="O52" s="94"/>
-      <c r="P52" s="94"/>
-      <c r="Q52" s="94"/>
-      <c r="R52" s="94"/>
-      <c r="S52" s="94"/>
-      <c r="T52" s="94"/>
-      <c r="U52" s="94"/>
-      <c r="V52" s="94"/>
-      <c r="W52" s="94"/>
-      <c r="X52" s="94"/>
-      <c r="Y52" s="94"/>
-      <c r="Z52" s="94"/>
-      <c r="AA52" s="95"/>
+      <c r="H52" s="96"/>
+      <c r="I52" s="96"/>
+      <c r="J52" s="96"/>
+      <c r="K52" s="96"/>
+      <c r="L52" s="96"/>
+      <c r="M52" s="96"/>
+      <c r="N52" s="96"/>
+      <c r="O52" s="96"/>
+      <c r="P52" s="96"/>
+      <c r="Q52" s="96"/>
+      <c r="R52" s="96"/>
+      <c r="S52" s="96"/>
+      <c r="T52" s="96"/>
+      <c r="U52" s="96"/>
+      <c r="V52" s="96"/>
+      <c r="W52" s="96"/>
+      <c r="X52" s="96"/>
+      <c r="Y52" s="96"/>
+      <c r="Z52" s="96"/>
+      <c r="AA52" s="97"/>
     </row>
     <row r="53" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="1048576" spans="16:16" x14ac:dyDescent="0.35">
@@ -3663,7 +3673,7 @@
   </sheetPr>
   <dimension ref="A1:AF1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="88" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="AD20" sqref="AD20"/>
     </sheetView>
   </sheetViews>
@@ -3681,115 +3691,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="105"/>
-      <c r="U1" s="105"/>
-      <c r="V1" s="105"/>
-      <c r="W1" s="105"/>
-      <c r="X1" s="105"/>
-      <c r="Y1" s="105"/>
-      <c r="Z1" s="105"/>
-      <c r="AA1" s="106"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="107"/>
+      <c r="T1" s="107"/>
+      <c r="U1" s="107"/>
+      <c r="V1" s="107"/>
+      <c r="W1" s="107"/>
+      <c r="X1" s="107"/>
+      <c r="Y1" s="107"/>
+      <c r="Z1" s="107"/>
+      <c r="AA1" s="108"/>
     </row>
     <row r="2" spans="1:32" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="102" t="s">
+      <c r="B2" s="101"/>
+      <c r="C2" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="107" t="s">
+      <c r="D2" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="111" t="s">
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="107"/>
-      <c r="S2" s="107"/>
-      <c r="T2" s="107"/>
-      <c r="U2" s="107"/>
-      <c r="V2" s="107"/>
-      <c r="W2" s="107"/>
-      <c r="X2" s="107"/>
-      <c r="Y2" s="107"/>
-      <c r="Z2" s="107"/>
-      <c r="AA2" s="112"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="109"/>
+      <c r="O2" s="109"/>
+      <c r="P2" s="109"/>
+      <c r="Q2" s="109"/>
+      <c r="R2" s="109"/>
+      <c r="S2" s="109"/>
+      <c r="T2" s="109"/>
+      <c r="U2" s="109"/>
+      <c r="V2" s="109"/>
+      <c r="W2" s="109"/>
+      <c r="X2" s="109"/>
+      <c r="Y2" s="109"/>
+      <c r="Z2" s="109"/>
+      <c r="AA2" s="114"/>
     </row>
     <row r="3" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="100"/>
-      <c r="B3" s="101"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="109"/>
-      <c r="E3" s="109"/>
-      <c r="F3" s="109"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="113" t="s">
+      <c r="A3" s="102"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="109"/>
-      <c r="J3" s="109"/>
-      <c r="K3" s="109"/>
-      <c r="L3" s="109"/>
-      <c r="M3" s="109" t="s">
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="109"/>
-      <c r="O3" s="109"/>
-      <c r="P3" s="109"/>
-      <c r="Q3" s="109"/>
-      <c r="R3" s="109" t="s">
+      <c r="N3" s="111"/>
+      <c r="O3" s="111"/>
+      <c r="P3" s="111"/>
+      <c r="Q3" s="111"/>
+      <c r="R3" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="109"/>
-      <c r="T3" s="109"/>
-      <c r="U3" s="109"/>
-      <c r="V3" s="109"/>
-      <c r="W3" s="109" t="s">
+      <c r="S3" s="111"/>
+      <c r="T3" s="111"/>
+      <c r="U3" s="111"/>
+      <c r="V3" s="111"/>
+      <c r="W3" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="109"/>
-      <c r="Y3" s="109"/>
-      <c r="Z3" s="109"/>
-      <c r="AA3" s="114"/>
+      <c r="X3" s="111"/>
+      <c r="Y3" s="111"/>
+      <c r="Z3" s="111"/>
+      <c r="AA3" s="116"/>
       <c r="AB3"/>
     </row>
     <row r="4" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="100"/>
-      <c r="B4" s="101"/>
-      <c r="C4" s="103"/>
+      <c r="A4" s="102"/>
+      <c r="B4" s="103"/>
+      <c r="C4" s="105"/>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
@@ -4308,12 +4318,12 @@
       <c r="C15" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="115"/>
-      <c r="E15" s="115"/>
-      <c r="F15" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="116"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="95"/>
       <c r="H15" s="50"/>
       <c r="I15" s="29"/>
       <c r="J15" s="29"/>
@@ -4349,12 +4359,12 @@
       <c r="C16" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="115"/>
-      <c r="E16" s="115"/>
-      <c r="F16" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="116"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="95"/>
       <c r="H16" s="50"/>
       <c r="I16" s="29"/>
       <c r="J16" s="56" t="s">
@@ -4392,12 +4402,12 @@
       <c r="C17" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="115"/>
-      <c r="E17" s="115"/>
-      <c r="F17" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="116"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="95"/>
       <c r="H17" s="50"/>
       <c r="I17" s="29"/>
       <c r="J17" s="29"/>
@@ -4433,12 +4443,12 @@
       <c r="C18" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="115"/>
-      <c r="E18" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="115"/>
-      <c r="G18" s="116"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="94"/>
+      <c r="G18" s="95"/>
       <c r="H18" s="50"/>
       <c r="I18" s="29"/>
       <c r="J18" s="57" t="s">
@@ -4472,12 +4482,12 @@
       <c r="C19" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="115"/>
-      <c r="E19" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="115"/>
-      <c r="G19" s="116"/>
+      <c r="D19" s="94"/>
+      <c r="E19" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="94"/>
+      <c r="G19" s="95"/>
       <c r="H19" s="50"/>
       <c r="I19" s="29"/>
       <c r="J19" s="57" t="s">
@@ -4513,12 +4523,12 @@
       <c r="C20" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="115"/>
-      <c r="E20" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="115"/>
-      <c r="G20" s="116"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="94"/>
+      <c r="G20" s="95"/>
       <c r="H20" s="50"/>
       <c r="I20" s="29"/>
       <c r="J20" s="57" t="s">
@@ -4554,10 +4564,10 @@
       <c r="C21" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="115"/>
-      <c r="E21" s="115"/>
-      <c r="F21" s="115"/>
-      <c r="G21" s="116" t="s">
+      <c r="D21" s="94"/>
+      <c r="E21" s="94"/>
+      <c r="F21" s="94"/>
+      <c r="G21" s="95" t="s">
         <v>12</v>
       </c>
       <c r="H21" s="50"/>
@@ -4595,10 +4605,10 @@
       <c r="C22" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="115"/>
-      <c r="E22" s="115"/>
-      <c r="F22" s="115"/>
-      <c r="G22" s="116" t="s">
+      <c r="D22" s="94"/>
+      <c r="E22" s="94"/>
+      <c r="F22" s="94"/>
+      <c r="G22" s="95" t="s">
         <v>12</v>
       </c>
       <c r="H22" s="50"/>
@@ -4636,10 +4646,10 @@
       <c r="C23" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="115"/>
-      <c r="E23" s="115"/>
-      <c r="F23" s="115"/>
-      <c r="G23" s="116" t="s">
+      <c r="D23" s="94"/>
+      <c r="E23" s="94"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="95" t="s">
         <v>12</v>
       </c>
       <c r="H23" s="50"/>
@@ -4677,12 +4687,12 @@
       <c r="C24" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="115"/>
-      <c r="F24" s="115"/>
-      <c r="G24" s="116"/>
+      <c r="D24" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="94"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="95"/>
       <c r="H24" s="50"/>
       <c r="I24" s="29"/>
       <c r="J24" s="58" t="s">
@@ -4716,12 +4726,12 @@
       <c r="C25" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="115"/>
-      <c r="E25" s="115"/>
-      <c r="F25" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="116"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="94"/>
+      <c r="F25" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="95"/>
       <c r="H25" s="50"/>
       <c r="I25" s="29"/>
       <c r="J25" s="29"/>
@@ -4755,12 +4765,12 @@
       <c r="C26" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="115"/>
-      <c r="F26" s="115"/>
-      <c r="G26" s="116"/>
+      <c r="D26" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="94"/>
+      <c r="F26" s="94"/>
+      <c r="G26" s="95"/>
       <c r="H26" s="50"/>
       <c r="I26" s="29"/>
       <c r="J26" s="29"/>
@@ -4794,12 +4804,12 @@
       <c r="C27" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="115"/>
-      <c r="F27" s="115"/>
-      <c r="G27" s="116"/>
+      <c r="D27" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="94"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="95"/>
       <c r="H27" s="50"/>
       <c r="I27" s="29"/>
       <c r="J27" s="29"/>
@@ -4833,10 +4843,10 @@
       <c r="C28" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="115"/>
-      <c r="E28" s="115"/>
-      <c r="F28" s="115"/>
-      <c r="G28" s="116" t="s">
+      <c r="D28" s="94"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="95" t="s">
         <v>12</v>
       </c>
       <c r="H28" s="50"/>
@@ -4872,12 +4882,12 @@
       <c r="C29" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="115"/>
-      <c r="E29" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="115"/>
-      <c r="G29" s="116"/>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="94"/>
+      <c r="G29" s="95"/>
       <c r="H29" s="50"/>
       <c r="I29" s="29"/>
       <c r="J29" s="29"/>
@@ -4911,12 +4921,12 @@
       <c r="C30" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="115"/>
-      <c r="E30" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="115"/>
-      <c r="G30" s="116"/>
+      <c r="D30" s="94"/>
+      <c r="E30" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="94"/>
+      <c r="G30" s="95"/>
       <c r="H30" s="50"/>
       <c r="I30" s="29"/>
       <c r="J30" s="29"/>
@@ -4952,10 +4962,10 @@
       <c r="C31" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="115"/>
-      <c r="E31" s="115"/>
-      <c r="F31" s="115"/>
-      <c r="G31" s="116" t="s">
+      <c r="D31" s="94"/>
+      <c r="E31" s="94"/>
+      <c r="F31" s="94"/>
+      <c r="G31" s="95" t="s">
         <v>12</v>
       </c>
       <c r="H31" s="50"/>
@@ -4991,10 +5001,10 @@
       <c r="C32" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="115"/>
-      <c r="E32" s="115"/>
-      <c r="F32" s="115"/>
-      <c r="G32" s="116" t="s">
+      <c r="D32" s="94"/>
+      <c r="E32" s="94"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="95" t="s">
         <v>12</v>
       </c>
       <c r="H32" s="50"/>
@@ -5032,10 +5042,10 @@
       <c r="C33" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="D33" s="115"/>
-      <c r="E33" s="115"/>
-      <c r="F33" s="115"/>
-      <c r="G33" s="116" t="s">
+      <c r="D33" s="94"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="94"/>
+      <c r="G33" s="95" t="s">
         <v>12</v>
       </c>
       <c r="H33" s="27"/>
@@ -5073,12 +5083,12 @@
       <c r="C34" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="115"/>
-      <c r="F34" s="115"/>
-      <c r="G34" s="116"/>
+      <c r="D34" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="94"/>
+      <c r="F34" s="94"/>
+      <c r="G34" s="95"/>
       <c r="H34" s="50"/>
       <c r="I34" s="29"/>
       <c r="J34" s="29"/>
@@ -5112,12 +5122,12 @@
       <c r="C35" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="115"/>
-      <c r="F35" s="115"/>
-      <c r="G35" s="116"/>
+      <c r="D35" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="94"/>
+      <c r="F35" s="94"/>
+      <c r="G35" s="95"/>
       <c r="H35" s="50"/>
       <c r="I35" s="29"/>
       <c r="J35" s="29"/>
@@ -5155,12 +5165,12 @@
       <c r="C36" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="115"/>
-      <c r="F36" s="115"/>
-      <c r="G36" s="116"/>
+      <c r="D36" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="94"/>
+      <c r="F36" s="94"/>
+      <c r="G36" s="95"/>
       <c r="H36" s="50"/>
       <c r="I36" s="29"/>
       <c r="J36" s="29"/>
@@ -5196,12 +5206,12 @@
       <c r="C37" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="115"/>
-      <c r="F37" s="115"/>
-      <c r="G37" s="116"/>
+      <c r="D37" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="94"/>
+      <c r="F37" s="94"/>
+      <c r="G37" s="95"/>
       <c r="H37" s="50"/>
       <c r="I37" s="29"/>
       <c r="J37" s="61" t="s">
@@ -5235,12 +5245,12 @@
       <c r="C38" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="115"/>
-      <c r="F38" s="115"/>
-      <c r="G38" s="116"/>
+      <c r="D38" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="94"/>
+      <c r="F38" s="94"/>
+      <c r="G38" s="95"/>
       <c r="H38" s="50"/>
       <c r="I38" s="29"/>
       <c r="J38" s="61" t="s">
@@ -5276,12 +5286,12 @@
       <c r="C39" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="D39" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" s="115"/>
-      <c r="F39" s="115"/>
-      <c r="G39" s="116"/>
+      <c r="D39" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="94"/>
+      <c r="F39" s="94"/>
+      <c r="G39" s="95"/>
       <c r="H39" s="50"/>
       <c r="I39" s="29"/>
       <c r="J39" s="61" t="s">
@@ -5317,12 +5327,12 @@
       <c r="C40" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="115"/>
-      <c r="E40" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="115"/>
-      <c r="G40" s="116"/>
+      <c r="D40" s="94"/>
+      <c r="E40" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="94"/>
+      <c r="G40" s="95"/>
       <c r="H40" s="50"/>
       <c r="I40" s="29"/>
       <c r="J40" s="29"/>
@@ -5356,12 +5366,12 @@
       <c r="C41" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="D41" s="115"/>
-      <c r="E41" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="F41" s="115"/>
-      <c r="G41" s="116"/>
+      <c r="D41" s="94"/>
+      <c r="E41" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="94"/>
+      <c r="G41" s="95"/>
       <c r="H41" s="50"/>
       <c r="I41" s="29"/>
       <c r="J41" s="29"/>
@@ -5397,12 +5407,12 @@
       <c r="C42" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="115"/>
-      <c r="E42" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="F42" s="115"/>
-      <c r="G42" s="116"/>
+      <c r="D42" s="94"/>
+      <c r="E42" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="94"/>
+      <c r="G42" s="95"/>
       <c r="H42" s="50"/>
       <c r="I42" s="29"/>
       <c r="J42" s="29"/>
@@ -5440,12 +5450,12 @@
       <c r="C43" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="D43" s="115"/>
-      <c r="E43" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" s="115"/>
-      <c r="G43" s="116"/>
+      <c r="D43" s="94"/>
+      <c r="E43" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="94"/>
+      <c r="G43" s="95"/>
       <c r="H43" s="50"/>
       <c r="I43" s="29"/>
       <c r="J43" s="29"/>
@@ -5481,12 +5491,12 @@
       <c r="C44" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="D44" s="115"/>
-      <c r="E44" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="F44" s="115"/>
-      <c r="G44" s="116"/>
+      <c r="D44" s="94"/>
+      <c r="E44" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="94"/>
+      <c r="G44" s="95"/>
       <c r="H44" s="50"/>
       <c r="I44" s="29"/>
       <c r="J44" s="29"/>
@@ -5524,12 +5534,12 @@
       <c r="C45" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="115"/>
-      <c r="E45" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45" s="115"/>
-      <c r="G45" s="116"/>
+      <c r="D45" s="94"/>
+      <c r="E45" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="94"/>
+      <c r="G45" s="95"/>
       <c r="H45" s="50"/>
       <c r="I45" s="29"/>
       <c r="J45" s="29"/>
@@ -5567,12 +5577,12 @@
       <c r="C46" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="D46" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" s="115"/>
-      <c r="F46" s="115"/>
-      <c r="G46" s="116"/>
+      <c r="D46" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="94"/>
+      <c r="F46" s="94"/>
+      <c r="G46" s="95"/>
       <c r="H46" s="50"/>
       <c r="I46" s="29"/>
       <c r="J46" s="29"/>
@@ -5606,12 +5616,12 @@
       <c r="C47" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="D47" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="E47" s="115"/>
-      <c r="F47" s="115"/>
-      <c r="G47" s="116"/>
+      <c r="D47" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="94"/>
+      <c r="F47" s="94"/>
+      <c r="G47" s="95"/>
       <c r="H47" s="50"/>
       <c r="I47" s="29"/>
       <c r="J47" s="29"/>
@@ -5647,12 +5657,12 @@
       <c r="C48" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="D48" s="115"/>
-      <c r="E48" s="115"/>
-      <c r="F48" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="G48" s="116" t="s">
+      <c r="D48" s="94"/>
+      <c r="E48" s="94"/>
+      <c r="F48" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" s="95" t="s">
         <v>12</v>
       </c>
       <c r="H48" s="27"/>
@@ -5686,16 +5696,16 @@
       <c r="C49" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="D49" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="F49" s="115" t="s">
-        <v>12</v>
-      </c>
-      <c r="G49" s="116" t="s">
+      <c r="D49" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" s="95" t="s">
         <v>12</v>
       </c>
       <c r="H49" s="51"/>
@@ -5802,8 +5812,8 @@
       <c r="AA51" s="73"/>
     </row>
     <row r="52" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="96"/>
-      <c r="B52" s="97"/>
+      <c r="A52" s="98"/>
+      <c r="B52" s="99"/>
       <c r="C52" s="74" t="s">
         <v>82</v>
       </c>
@@ -5823,26 +5833,2236 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H52" s="94"/>
-      <c r="I52" s="94"/>
-      <c r="J52" s="94"/>
-      <c r="K52" s="94"/>
-      <c r="L52" s="94"/>
-      <c r="M52" s="94"/>
-      <c r="N52" s="94"/>
-      <c r="O52" s="94"/>
-      <c r="P52" s="94"/>
-      <c r="Q52" s="94"/>
-      <c r="R52" s="94"/>
-      <c r="S52" s="94"/>
-      <c r="T52" s="94"/>
-      <c r="U52" s="94"/>
-      <c r="V52" s="94"/>
-      <c r="W52" s="94"/>
-      <c r="X52" s="94"/>
-      <c r="Y52" s="94"/>
-      <c r="Z52" s="94"/>
-      <c r="AA52" s="95"/>
+      <c r="H52" s="96"/>
+      <c r="I52" s="96"/>
+      <c r="J52" s="96"/>
+      <c r="K52" s="96"/>
+      <c r="L52" s="96"/>
+      <c r="M52" s="96"/>
+      <c r="N52" s="96"/>
+      <c r="O52" s="96"/>
+      <c r="P52" s="96"/>
+      <c r="Q52" s="96"/>
+      <c r="R52" s="96"/>
+      <c r="S52" s="96"/>
+      <c r="T52" s="96"/>
+      <c r="U52" s="96"/>
+      <c r="V52" s="96"/>
+      <c r="W52" s="96"/>
+      <c r="X52" s="96"/>
+      <c r="Y52" s="96"/>
+      <c r="Z52" s="96"/>
+      <c r="AA52" s="97"/>
+    </row>
+    <row r="53" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="1048576" spans="16:16" x14ac:dyDescent="0.35">
+      <c r="P1048576" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="H52:AA52"/>
+    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="A2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="H2:AA2"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="R3:V3"/>
+    <mergeCell ref="W3:AA3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85C60A3-BA5A-4630-A380-9EAD816EDB68}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:AF1048576"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="88" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.6328125" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="17" width="2.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="26" width="2.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="2.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.90625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="107"/>
+      <c r="T1" s="107"/>
+      <c r="U1" s="107"/>
+      <c r="V1" s="107"/>
+      <c r="W1" s="107"/>
+      <c r="X1" s="107"/>
+      <c r="Y1" s="107"/>
+      <c r="Z1" s="107"/>
+      <c r="AA1" s="108"/>
+    </row>
+    <row r="2" spans="1:32" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="100" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="101"/>
+      <c r="C2" s="104" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="109" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="113" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="109"/>
+      <c r="O2" s="109"/>
+      <c r="P2" s="109"/>
+      <c r="Q2" s="109"/>
+      <c r="R2" s="109"/>
+      <c r="S2" s="109"/>
+      <c r="T2" s="109"/>
+      <c r="U2" s="109"/>
+      <c r="V2" s="109"/>
+      <c r="W2" s="109"/>
+      <c r="X2" s="109"/>
+      <c r="Y2" s="109"/>
+      <c r="Z2" s="109"/>
+      <c r="AA2" s="114"/>
+    </row>
+    <row r="3" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="102"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="115" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="111"/>
+      <c r="J3" s="111"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="111" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="111"/>
+      <c r="O3" s="111"/>
+      <c r="P3" s="111"/>
+      <c r="Q3" s="111"/>
+      <c r="R3" s="111" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" s="111"/>
+      <c r="T3" s="111"/>
+      <c r="U3" s="111"/>
+      <c r="V3" s="111"/>
+      <c r="W3" s="111" t="s">
+        <v>7</v>
+      </c>
+      <c r="X3" s="111"/>
+      <c r="Y3" s="111"/>
+      <c r="Z3" s="111"/>
+      <c r="AA3" s="116"/>
+      <c r="AB3"/>
+    </row>
+    <row r="4" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="102"/>
+      <c r="B4" s="103"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="27">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1">
+        <v>4</v>
+      </c>
+      <c r="L4" s="1">
+        <v>5</v>
+      </c>
+      <c r="M4" s="1">
+        <v>6</v>
+      </c>
+      <c r="N4" s="1">
+        <v>7</v>
+      </c>
+      <c r="O4" s="1">
+        <v>8</v>
+      </c>
+      <c r="P4" s="1">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>10</v>
+      </c>
+      <c r="R4" s="1">
+        <v>11</v>
+      </c>
+      <c r="S4" s="1">
+        <v>12</v>
+      </c>
+      <c r="T4" s="1">
+        <v>13</v>
+      </c>
+      <c r="U4" s="1">
+        <v>14</v>
+      </c>
+      <c r="V4" s="1">
+        <v>15</v>
+      </c>
+      <c r="W4" s="1">
+        <v>16</v>
+      </c>
+      <c r="X4" s="1">
+        <v>17</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>18</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>19</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>20</v>
+      </c>
+      <c r="AB4"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="34">
+        <v>1</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5"/>
+      <c r="AC5"/>
+      <c r="AD5"/>
+      <c r="AE5"/>
+      <c r="AF5"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="35">
+        <v>1</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="50"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="76"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="54"/>
+      <c r="T6" s="54"/>
+      <c r="U6" s="54"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="29"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="28"/>
+      <c r="AB6"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="35">
+        <v>2</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="93" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="93" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="28"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="35">
+        <v>3</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="50"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="28"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="29"/>
+      <c r="W8" s="29"/>
+      <c r="X8" s="29"/>
+      <c r="Y8" s="29"/>
+      <c r="Z8" s="29"/>
+      <c r="AA8" s="28"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="36">
+        <v>1</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="50"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="77" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" s="28"/>
+      <c r="N9" s="50"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q9" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="R9" s="29"/>
+      <c r="S9" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="T9" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="U9" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="V9" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="W9" s="29"/>
+      <c r="X9" s="29"/>
+      <c r="Y9" s="29"/>
+      <c r="Z9" s="29"/>
+      <c r="AA9" s="28"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="36">
+        <v>2</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="50"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="77" t="s">
+        <v>38</v>
+      </c>
+      <c r="M10" s="28"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="W10" s="29"/>
+      <c r="X10" s="29"/>
+      <c r="Y10" s="29"/>
+      <c r="Z10" s="29"/>
+      <c r="AA10" s="28"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A11" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="37">
+        <v>1</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="52"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="29"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="29"/>
+      <c r="V11" s="29"/>
+      <c r="W11" s="29"/>
+      <c r="X11" s="29"/>
+      <c r="Y11" s="29"/>
+      <c r="Z11" s="29"/>
+      <c r="AA11" s="28"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A12" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="37">
+        <v>2</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="52"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" s="50"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="29"/>
+      <c r="T12" s="29"/>
+      <c r="U12" s="29"/>
+      <c r="V12" s="29"/>
+      <c r="W12" s="29"/>
+      <c r="X12" s="29"/>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="29"/>
+      <c r="AA12" s="28"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A13" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="37">
+        <v>3</v>
+      </c>
+      <c r="C13" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="52"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="50"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29"/>
+      <c r="T13" s="29"/>
+      <c r="U13" s="29"/>
+      <c r="V13" s="29"/>
+      <c r="W13" s="29"/>
+      <c r="X13" s="29"/>
+      <c r="Y13" s="29"/>
+      <c r="Z13" s="29"/>
+      <c r="AA13" s="28"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A14" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="37">
+        <v>4</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="52"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="M14" s="28"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="29"/>
+      <c r="U14" s="29"/>
+      <c r="V14" s="29"/>
+      <c r="W14" s="29"/>
+      <c r="X14" s="29"/>
+      <c r="Y14" s="29"/>
+      <c r="Z14" s="29"/>
+      <c r="AA14" s="28"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A15" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="37">
+        <v>5</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="95"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="M15" s="28"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29"/>
+      <c r="T15" s="29"/>
+      <c r="U15" s="29"/>
+      <c r="V15" s="29"/>
+      <c r="W15" s="29"/>
+      <c r="X15" s="29"/>
+      <c r="Y15" s="29"/>
+      <c r="Z15" s="29"/>
+      <c r="AA15" s="28"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A16" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="37">
+        <v>6</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="94"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="95"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="M16" s="28"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="29"/>
+      <c r="S16" s="29"/>
+      <c r="T16" s="29"/>
+      <c r="U16" s="29"/>
+      <c r="V16" s="29"/>
+      <c r="W16" s="29"/>
+      <c r="X16" s="29"/>
+      <c r="Y16" s="29"/>
+      <c r="Z16" s="29"/>
+      <c r="AA16" s="28"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="38">
+        <v>1</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="94"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="95"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="M17" s="85" t="s">
+        <v>38</v>
+      </c>
+      <c r="N17" s="50"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="29"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="29"/>
+      <c r="AA17" s="28"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="34">
+        <v>1</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="94"/>
+      <c r="E18" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="94"/>
+      <c r="G18" s="95"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="29"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
+      <c r="T18" s="29"/>
+      <c r="U18" s="29"/>
+      <c r="V18" s="29"/>
+      <c r="W18" s="29"/>
+      <c r="X18" s="29"/>
+      <c r="Y18" s="29"/>
+      <c r="Z18" s="29"/>
+      <c r="AA18" s="28"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="34">
+        <v>2</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="94"/>
+      <c r="E19" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="94"/>
+      <c r="G19" s="95"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" s="50"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="29"/>
+      <c r="V19" s="29"/>
+      <c r="W19" s="29"/>
+      <c r="X19" s="29"/>
+      <c r="Y19" s="29"/>
+      <c r="Z19" s="29"/>
+      <c r="AA19" s="28"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="34">
+        <v>3</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="94"/>
+      <c r="E20" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="94"/>
+      <c r="G20" s="95"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" s="50"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29"/>
+      <c r="T20" s="29"/>
+      <c r="U20" s="29"/>
+      <c r="V20" s="29"/>
+      <c r="W20" s="29"/>
+      <c r="X20" s="29"/>
+      <c r="Y20" s="29"/>
+      <c r="Z20" s="29"/>
+      <c r="AA20" s="28"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="34">
+        <v>4</v>
+      </c>
+      <c r="C21" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="94"/>
+      <c r="E21" s="94"/>
+      <c r="F21" s="94"/>
+      <c r="G21" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="50"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" s="50"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="U21" s="29"/>
+      <c r="V21" s="29"/>
+      <c r="W21" s="29"/>
+      <c r="X21" s="29"/>
+      <c r="Y21" s="29"/>
+      <c r="Z21" s="29"/>
+      <c r="AA21" s="28"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="34">
+        <v>5</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="94"/>
+      <c r="E22" s="94"/>
+      <c r="F22" s="94"/>
+      <c r="G22" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="50"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="L22" s="50"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="29"/>
+      <c r="T22" s="29"/>
+      <c r="U22" s="29"/>
+      <c r="V22" s="29"/>
+      <c r="W22" s="29"/>
+      <c r="X22" s="29"/>
+      <c r="Y22" s="29"/>
+      <c r="Z22" s="29"/>
+      <c r="AA22" s="28"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="34">
+        <v>6</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="94"/>
+      <c r="E23" s="94"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="50"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="L23" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="M23" s="28"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="29"/>
+      <c r="T23" s="29"/>
+      <c r="U23" s="29"/>
+      <c r="V23" s="29"/>
+      <c r="W23" s="29"/>
+      <c r="X23" s="29"/>
+      <c r="Y23" s="29"/>
+      <c r="Z23" s="29"/>
+      <c r="AA23" s="28"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="39">
+        <v>1</v>
+      </c>
+      <c r="C24" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="94"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" s="29"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="29"/>
+      <c r="T24" s="29"/>
+      <c r="U24" s="29"/>
+      <c r="V24" s="29"/>
+      <c r="W24" s="29"/>
+      <c r="X24" s="29"/>
+      <c r="Y24" s="29"/>
+      <c r="Z24" s="29"/>
+      <c r="AA24" s="28"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="39">
+        <v>2</v>
+      </c>
+      <c r="C25" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="94"/>
+      <c r="E25" s="94"/>
+      <c r="F25" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="95"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="50"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="29"/>
+      <c r="S25" s="29"/>
+      <c r="T25" s="29"/>
+      <c r="U25" s="29"/>
+      <c r="V25" s="29"/>
+      <c r="W25" s="29"/>
+      <c r="X25" s="29"/>
+      <c r="Y25" s="29"/>
+      <c r="Z25" s="29"/>
+      <c r="AA25" s="28"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A26" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="39">
+        <v>3</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="94"/>
+      <c r="F26" s="94"/>
+      <c r="G26" s="95"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="91" t="s">
+        <v>8</v>
+      </c>
+      <c r="O26" s="29"/>
+      <c r="P26" s="29"/>
+      <c r="Q26" s="29"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="29"/>
+      <c r="T26" s="29"/>
+      <c r="U26" s="29"/>
+      <c r="V26" s="29"/>
+      <c r="W26" s="29"/>
+      <c r="X26" s="29"/>
+      <c r="Y26" s="29"/>
+      <c r="Z26" s="29"/>
+      <c r="AA26" s="28"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A27" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="39">
+        <v>4</v>
+      </c>
+      <c r="C27" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="94"/>
+      <c r="F27" s="94"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="119" t="s">
+        <v>8</v>
+      </c>
+      <c r="N27" s="50"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="29"/>
+      <c r="T27" s="29"/>
+      <c r="U27" s="29"/>
+      <c r="V27" s="29"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
+      <c r="Y27" s="29"/>
+      <c r="Z27" s="29"/>
+      <c r="AA27" s="28"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A28" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="40">
+        <v>1</v>
+      </c>
+      <c r="C28" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="94"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="50"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="120" t="s">
+        <v>39</v>
+      </c>
+      <c r="N28" s="50"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29"/>
+      <c r="Q28" s="29"/>
+      <c r="R28" s="29"/>
+      <c r="S28" s="29"/>
+      <c r="T28" s="29"/>
+      <c r="U28" s="29"/>
+      <c r="V28" s="29"/>
+      <c r="W28" s="29"/>
+      <c r="X28" s="29"/>
+      <c r="Y28" s="29"/>
+      <c r="Z28" s="29"/>
+      <c r="AA28" s="28"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A29" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="41">
+        <v>1</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="94"/>
+      <c r="G29" s="95"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="80" t="s">
+        <v>9</v>
+      </c>
+      <c r="M29" s="28"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="29"/>
+      <c r="Q29" s="29"/>
+      <c r="R29" s="29"/>
+      <c r="S29" s="29"/>
+      <c r="T29" s="29"/>
+      <c r="U29" s="29"/>
+      <c r="V29" s="29"/>
+      <c r="W29" s="29"/>
+      <c r="X29" s="29"/>
+      <c r="Y29" s="29"/>
+      <c r="Z29" s="29"/>
+      <c r="AA29" s="28"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A30" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="41">
+        <v>2</v>
+      </c>
+      <c r="C30" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="94"/>
+      <c r="E30" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="94"/>
+      <c r="G30" s="95"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="80" t="s">
+        <v>9</v>
+      </c>
+      <c r="M30" s="121" t="s">
+        <v>9</v>
+      </c>
+      <c r="N30" s="50"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="29"/>
+      <c r="Q30" s="29"/>
+      <c r="R30" s="29"/>
+      <c r="S30" s="29"/>
+      <c r="T30" s="29"/>
+      <c r="U30" s="29"/>
+      <c r="V30" s="29"/>
+      <c r="W30" s="29"/>
+      <c r="X30" s="29"/>
+      <c r="Y30" s="29"/>
+      <c r="Z30" s="29"/>
+      <c r="AA30" s="28"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A31" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="42">
+        <v>1</v>
+      </c>
+      <c r="C31" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="94"/>
+      <c r="E31" s="94"/>
+      <c r="F31" s="94"/>
+      <c r="G31" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="50"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="K31" s="29"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="28"/>
+      <c r="N31" s="50"/>
+      <c r="O31" s="29"/>
+      <c r="P31" s="29"/>
+      <c r="Q31" s="29"/>
+      <c r="R31" s="29"/>
+      <c r="S31" s="29"/>
+      <c r="T31" s="29"/>
+      <c r="U31" s="29"/>
+      <c r="V31" s="29"/>
+      <c r="W31" s="29"/>
+      <c r="X31" s="29"/>
+      <c r="Y31" s="29"/>
+      <c r="Z31" s="29"/>
+      <c r="AA31" s="28"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A32" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="42">
+        <v>2</v>
+      </c>
+      <c r="C32" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="94"/>
+      <c r="E32" s="94"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="50"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="L32" s="81" t="s">
+        <v>39</v>
+      </c>
+      <c r="M32" s="28"/>
+      <c r="N32" s="50"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="29"/>
+      <c r="Q32" s="29"/>
+      <c r="R32" s="29"/>
+      <c r="S32" s="29"/>
+      <c r="T32" s="29"/>
+      <c r="U32" s="29"/>
+      <c r="V32" s="29"/>
+      <c r="W32" s="29"/>
+      <c r="X32" s="29"/>
+      <c r="Y32" s="29"/>
+      <c r="Z32" s="29"/>
+      <c r="AA32" s="28"/>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="42">
+        <v>3</v>
+      </c>
+      <c r="C33" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="94"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="94"/>
+      <c r="G33" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="27"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="81" t="s">
+        <v>39</v>
+      </c>
+      <c r="M33" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="N33" s="27"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="2"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A34" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="42">
+        <v>4</v>
+      </c>
+      <c r="C34" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="94"/>
+      <c r="F34" s="94"/>
+      <c r="G34" s="95"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="50"/>
+      <c r="M34" s="87" t="s">
+        <v>8</v>
+      </c>
+      <c r="N34" s="50"/>
+      <c r="O34" s="29"/>
+      <c r="P34" s="29"/>
+      <c r="Q34" s="29"/>
+      <c r="R34" s="29"/>
+      <c r="S34" s="29"/>
+      <c r="T34" s="29"/>
+      <c r="U34" s="29"/>
+      <c r="V34" s="29"/>
+      <c r="W34" s="29"/>
+      <c r="X34" s="29"/>
+      <c r="Y34" s="29"/>
+      <c r="Z34" s="29"/>
+      <c r="AA34" s="28"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A35" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="42">
+        <v>5</v>
+      </c>
+      <c r="C35" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="94"/>
+      <c r="F35" s="94"/>
+      <c r="G35" s="95"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="50"/>
+      <c r="M35" s="87" t="s">
+        <v>8</v>
+      </c>
+      <c r="N35" s="81" t="s">
+        <v>8</v>
+      </c>
+      <c r="O35" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="P35" s="29"/>
+      <c r="Q35" s="29"/>
+      <c r="R35" s="29"/>
+      <c r="S35" s="29"/>
+      <c r="T35" s="29"/>
+      <c r="U35" s="29"/>
+      <c r="V35" s="29"/>
+      <c r="W35" s="29"/>
+      <c r="X35" s="29"/>
+      <c r="Y35" s="29"/>
+      <c r="Z35" s="29"/>
+      <c r="AA35" s="28"/>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A36" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="42">
+        <v>6</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="94"/>
+      <c r="F36" s="94"/>
+      <c r="G36" s="95"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="50"/>
+      <c r="M36" s="28"/>
+      <c r="N36" s="81" t="s">
+        <v>8</v>
+      </c>
+      <c r="O36" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="P36" s="29"/>
+      <c r="Q36" s="29"/>
+      <c r="R36" s="29"/>
+      <c r="S36" s="29"/>
+      <c r="T36" s="29"/>
+      <c r="U36" s="29"/>
+      <c r="V36" s="29"/>
+      <c r="W36" s="29"/>
+      <c r="X36" s="29"/>
+      <c r="Y36" s="29"/>
+      <c r="Z36" s="29"/>
+      <c r="AA36" s="28"/>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A37" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="43">
+        <v>1</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="94"/>
+      <c r="F37" s="94"/>
+      <c r="G37" s="95"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="K37" s="29"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="28"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="29"/>
+      <c r="T37" s="29"/>
+      <c r="U37" s="29"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="29"/>
+      <c r="Y37" s="29"/>
+      <c r="Z37" s="29"/>
+      <c r="AA37" s="28"/>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A38" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="43">
+        <v>2</v>
+      </c>
+      <c r="C38" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="94"/>
+      <c r="F38" s="94"/>
+      <c r="G38" s="95"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="K38" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="L38" s="50"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+      <c r="T38" s="29"/>
+      <c r="U38" s="29"/>
+      <c r="V38" s="29"/>
+      <c r="W38" s="29"/>
+      <c r="X38" s="29"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
+      <c r="AA38" s="28"/>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A39" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="43">
+        <v>3</v>
+      </c>
+      <c r="C39" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="94"/>
+      <c r="F39" s="94"/>
+      <c r="G39" s="95"/>
+      <c r="H39" s="50"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="K39" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="L39" s="50"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="50"/>
+      <c r="O39" s="29"/>
+      <c r="P39" s="29"/>
+      <c r="Q39" s="29"/>
+      <c r="R39" s="29"/>
+      <c r="S39" s="29"/>
+      <c r="T39" s="29"/>
+      <c r="U39" s="29"/>
+      <c r="V39" s="29"/>
+      <c r="W39" s="29"/>
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="28"/>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A40" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="44">
+        <v>1</v>
+      </c>
+      <c r="C40" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="94"/>
+      <c r="E40" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="94"/>
+      <c r="G40" s="95"/>
+      <c r="H40" s="50"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="50"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="117" t="s">
+        <v>9</v>
+      </c>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="29"/>
+      <c r="R40" s="29"/>
+      <c r="S40" s="29"/>
+      <c r="T40" s="29"/>
+      <c r="U40" s="29"/>
+      <c r="V40" s="29"/>
+      <c r="W40" s="29"/>
+      <c r="X40" s="29"/>
+      <c r="Y40" s="29"/>
+      <c r="Z40" s="29"/>
+      <c r="AA40" s="28"/>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A41" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="44">
+        <v>2</v>
+      </c>
+      <c r="C41" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" s="94"/>
+      <c r="E41" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="94"/>
+      <c r="G41" s="95"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="29"/>
+      <c r="L41" s="50"/>
+      <c r="M41" s="28"/>
+      <c r="N41" s="117" t="s">
+        <v>9</v>
+      </c>
+      <c r="O41" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P41" s="29"/>
+      <c r="Q41" s="29"/>
+      <c r="R41" s="29"/>
+      <c r="S41" s="29"/>
+      <c r="T41" s="29"/>
+      <c r="U41" s="29"/>
+      <c r="V41" s="29"/>
+      <c r="W41" s="29"/>
+      <c r="X41" s="29"/>
+      <c r="Y41" s="29"/>
+      <c r="Z41" s="29"/>
+      <c r="AA41" s="28"/>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A42" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="44">
+        <v>3</v>
+      </c>
+      <c r="C42" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="94"/>
+      <c r="E42" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="94"/>
+      <c r="G42" s="95"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="50"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="50"/>
+      <c r="O42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="P42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="R42" s="29"/>
+      <c r="S42" s="29"/>
+      <c r="T42" s="29"/>
+      <c r="U42" s="29"/>
+      <c r="V42" s="29"/>
+      <c r="W42" s="29"/>
+      <c r="X42" s="29"/>
+      <c r="Y42" s="29"/>
+      <c r="Z42" s="29"/>
+      <c r="AA42" s="28"/>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A43" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="45">
+        <v>1</v>
+      </c>
+      <c r="C43" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="94"/>
+      <c r="E43" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="94"/>
+      <c r="G43" s="95"/>
+      <c r="H43" s="50"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="50"/>
+      <c r="M43" s="28"/>
+      <c r="N43" s="50"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q43" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="R43" s="29"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="29"/>
+      <c r="U43" s="29"/>
+      <c r="V43" s="29"/>
+      <c r="W43" s="29"/>
+      <c r="X43" s="29"/>
+      <c r="Y43" s="29"/>
+      <c r="Z43" s="29"/>
+      <c r="AA43" s="28"/>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A44" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="45">
+        <v>2</v>
+      </c>
+      <c r="C44" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="94"/>
+      <c r="E44" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="94"/>
+      <c r="G44" s="95"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="50"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q44" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="R44" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="S44" s="29"/>
+      <c r="T44" s="29"/>
+      <c r="U44" s="29"/>
+      <c r="V44" s="29"/>
+      <c r="W44" s="29"/>
+      <c r="X44" s="29"/>
+      <c r="Y44" s="29"/>
+      <c r="Z44" s="29"/>
+      <c r="AA44" s="28"/>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A45" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="45">
+        <v>3</v>
+      </c>
+      <c r="C45" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="94"/>
+      <c r="E45" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="94"/>
+      <c r="G45" s="95"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="29"/>
+      <c r="L45" s="50"/>
+      <c r="M45" s="28"/>
+      <c r="N45" s="50"/>
+      <c r="O45" s="29"/>
+      <c r="P45" s="29"/>
+      <c r="Q45" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="R45" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="S45" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="T45" s="29"/>
+      <c r="U45" s="29"/>
+      <c r="V45" s="29"/>
+      <c r="W45" s="29"/>
+      <c r="X45" s="29"/>
+      <c r="Y45" s="29"/>
+      <c r="Z45" s="29"/>
+      <c r="AA45" s="28"/>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A46" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="46">
+        <v>1</v>
+      </c>
+      <c r="C46" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="94"/>
+      <c r="F46" s="94"/>
+      <c r="G46" s="95"/>
+      <c r="H46" s="50"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
+      <c r="K46" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="L46" s="50"/>
+      <c r="M46" s="28"/>
+      <c r="N46" s="50"/>
+      <c r="O46" s="29"/>
+      <c r="P46" s="29"/>
+      <c r="Q46" s="29"/>
+      <c r="R46" s="29"/>
+      <c r="S46" s="29"/>
+      <c r="T46" s="29"/>
+      <c r="U46" s="29"/>
+      <c r="V46" s="29"/>
+      <c r="W46" s="29"/>
+      <c r="X46" s="29"/>
+      <c r="Y46" s="29"/>
+      <c r="Z46" s="29"/>
+      <c r="AA46" s="28"/>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A47" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="46">
+        <v>2</v>
+      </c>
+      <c r="C47" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="94"/>
+      <c r="F47" s="94"/>
+      <c r="G47" s="95"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
+      <c r="K47" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="L47" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="M47" s="28"/>
+      <c r="N47" s="50"/>
+      <c r="O47" s="29"/>
+      <c r="P47" s="29"/>
+      <c r="Q47" s="29"/>
+      <c r="R47" s="29"/>
+      <c r="S47" s="29"/>
+      <c r="T47" s="29"/>
+      <c r="U47" s="29"/>
+      <c r="V47" s="29"/>
+      <c r="W47" s="29"/>
+      <c r="X47" s="29"/>
+      <c r="Y47" s="29"/>
+      <c r="Z47" s="29"/>
+      <c r="AA47" s="28"/>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A48" s="65" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="64">
+        <v>1</v>
+      </c>
+      <c r="C48" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="94"/>
+      <c r="E48" s="94"/>
+      <c r="F48" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" s="27"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="27"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="118"/>
+      <c r="O48" s="65"/>
+      <c r="P48" s="65"/>
+      <c r="Q48" s="65"/>
+      <c r="R48" s="65"/>
+      <c r="S48" s="65"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
+      <c r="X48" s="1"/>
+      <c r="Y48" s="1"/>
+      <c r="Z48" s="1"/>
+      <c r="AA48" s="2"/>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A49" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="47">
+        <v>1</v>
+      </c>
+      <c r="C49" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" s="51"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="31"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="51"/>
+      <c r="M49" s="90"/>
+      <c r="N49" s="51"/>
+      <c r="O49" s="31"/>
+      <c r="P49" s="31"/>
+      <c r="Q49" s="31"/>
+      <c r="R49" s="31"/>
+      <c r="S49" s="31"/>
+      <c r="T49" s="31"/>
+      <c r="U49" s="31"/>
+      <c r="V49" s="31"/>
+      <c r="W49" s="31"/>
+      <c r="X49" s="29"/>
+      <c r="Y49" s="29"/>
+      <c r="Z49" s="29"/>
+      <c r="AA49" s="28"/>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A50" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" s="48">
+        <v>1</v>
+      </c>
+      <c r="C50" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" s="50"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="29"/>
+      <c r="L50" s="50"/>
+      <c r="M50" s="28"/>
+      <c r="N50" s="50"/>
+      <c r="O50" s="29"/>
+      <c r="P50" s="29"/>
+      <c r="Q50" s="29"/>
+      <c r="R50" s="29"/>
+      <c r="S50" s="29"/>
+      <c r="T50" s="53"/>
+      <c r="U50" s="53"/>
+      <c r="V50" s="53"/>
+      <c r="W50" s="53"/>
+      <c r="X50" s="29"/>
+      <c r="Y50" s="29"/>
+      <c r="Z50" s="29"/>
+      <c r="AA50" s="28"/>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A51" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51" s="67">
+        <v>1</v>
+      </c>
+      <c r="C51" s="68" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="69"/>
+      <c r="H51" s="70"/>
+      <c r="I51" s="71"/>
+      <c r="J51" s="71"/>
+      <c r="K51" s="29"/>
+      <c r="L51" s="70"/>
+      <c r="M51" s="28"/>
+      <c r="N51" s="70"/>
+      <c r="O51" s="71"/>
+      <c r="P51" s="71"/>
+      <c r="Q51" s="71"/>
+      <c r="R51" s="71"/>
+      <c r="S51" s="71"/>
+      <c r="T51" s="71"/>
+      <c r="U51" s="71"/>
+      <c r="V51" s="71"/>
+      <c r="W51" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="X51" s="71"/>
+      <c r="Y51" s="71"/>
+      <c r="Z51" s="71"/>
+      <c r="AA51" s="73"/>
+    </row>
+    <row r="52" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="98"/>
+      <c r="B52" s="99"/>
+      <c r="C52" s="74" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" s="30">
+        <f t="shared" ref="D52:G52" si="0">COUNTIF(D5:D51, "X")</f>
+        <v>17</v>
+      </c>
+      <c r="E52" s="30">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F52" s="30">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G52" s="30">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="H52" s="96"/>
+      <c r="I52" s="96"/>
+      <c r="J52" s="96"/>
+      <c r="K52" s="96"/>
+      <c r="L52" s="96"/>
+      <c r="M52" s="96"/>
+      <c r="N52" s="96"/>
+      <c r="O52" s="96"/>
+      <c r="P52" s="96"/>
+      <c r="Q52" s="96"/>
+      <c r="R52" s="96"/>
+      <c r="S52" s="96"/>
+      <c r="T52" s="96"/>
+      <c r="U52" s="96"/>
+      <c r="V52" s="96"/>
+      <c r="W52" s="96"/>
+      <c r="X52" s="96"/>
+      <c r="Y52" s="96"/>
+      <c r="Z52" s="96"/>
+      <c r="AA52" s="97"/>
     </row>
     <row r="53" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="1048576" spans="16:16" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Apañao  Gantt Diagram final edition
</commit_message>
<xml_diff>
--- a/Reuniones_Coordinacion/I3_Gant_D1_Saul_Fernando_Raquel_Irene.xlsx
+++ b/Reuniones_Coordinacion/I3_Gant_D1_Saul_Fernando_Raquel_Irene.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\saul\Pprog_conversation\Reuniones_Coordinacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437CBA5B-5BB2-4783-9B91-0EE97D674BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D557C49-966A-4DA8-877C-7813C2EEC67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{05C49126-5558-4AD1-950B-328547F3A5DA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{05C49126-5558-4AD1-950B-328547F3A5DA}"/>
   </bookViews>
   <sheets>
     <sheet name="ASIGNACIÓN DE RECURSOS" sheetId="2" r:id="rId1"/>
@@ -891,7 +891,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1189,6 +1189,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1250,12 +1253,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1647,7 +1644,7 @@
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
@@ -1665,115 +1662,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="166" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="166"/>
-      <c r="S1" s="166"/>
-      <c r="T1" s="166"/>
-      <c r="U1" s="166"/>
-      <c r="V1" s="166"/>
-      <c r="W1" s="166"/>
-      <c r="X1" s="166"/>
-      <c r="Y1" s="166"/>
-      <c r="Z1" s="166"/>
-      <c r="AA1" s="167"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
+      <c r="P1" s="167"/>
+      <c r="Q1" s="167"/>
+      <c r="R1" s="167"/>
+      <c r="S1" s="167"/>
+      <c r="T1" s="167"/>
+      <c r="U1" s="167"/>
+      <c r="V1" s="167"/>
+      <c r="W1" s="167"/>
+      <c r="X1" s="167"/>
+      <c r="Y1" s="167"/>
+      <c r="Z1" s="167"/>
+      <c r="AA1" s="168"/>
     </row>
     <row r="2" spans="1:28" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="160"/>
-      <c r="C2" s="163" t="s">
+      <c r="B2" s="161"/>
+      <c r="C2" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="168" t="s">
+      <c r="D2" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="168"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="172" t="s">
+      <c r="E2" s="169"/>
+      <c r="F2" s="169"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="173" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="168"/>
-      <c r="J2" s="168"/>
-      <c r="K2" s="168"/>
-      <c r="L2" s="168"/>
-      <c r="M2" s="168"/>
-      <c r="N2" s="168"/>
-      <c r="O2" s="168"/>
-      <c r="P2" s="168"/>
-      <c r="Q2" s="168"/>
-      <c r="R2" s="168"/>
-      <c r="S2" s="168"/>
-      <c r="T2" s="168"/>
-      <c r="U2" s="168"/>
-      <c r="V2" s="168"/>
-      <c r="W2" s="168"/>
-      <c r="X2" s="168"/>
-      <c r="Y2" s="168"/>
-      <c r="Z2" s="168"/>
-      <c r="AA2" s="173"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="169"/>
+      <c r="K2" s="169"/>
+      <c r="L2" s="169"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
+      <c r="O2" s="169"/>
+      <c r="P2" s="169"/>
+      <c r="Q2" s="169"/>
+      <c r="R2" s="169"/>
+      <c r="S2" s="169"/>
+      <c r="T2" s="169"/>
+      <c r="U2" s="169"/>
+      <c r="V2" s="169"/>
+      <c r="W2" s="169"/>
+      <c r="X2" s="169"/>
+      <c r="Y2" s="169"/>
+      <c r="Z2" s="169"/>
+      <c r="AA2" s="174"/>
     </row>
     <row r="3" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="161"/>
-      <c r="B3" s="162"/>
-      <c r="C3" s="164"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="174" t="s">
+      <c r="A3" s="162"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="171"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="171"/>
+      <c r="G3" s="172"/>
+      <c r="H3" s="175" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="170"/>
-      <c r="J3" s="170"/>
-      <c r="K3" s="170"/>
-      <c r="L3" s="170"/>
-      <c r="M3" s="170" t="s">
+      <c r="I3" s="171"/>
+      <c r="J3" s="171"/>
+      <c r="K3" s="171"/>
+      <c r="L3" s="171"/>
+      <c r="M3" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="170"/>
-      <c r="O3" s="170"/>
-      <c r="P3" s="170"/>
-      <c r="Q3" s="170"/>
-      <c r="R3" s="170" t="s">
+      <c r="N3" s="171"/>
+      <c r="O3" s="171"/>
+      <c r="P3" s="171"/>
+      <c r="Q3" s="171"/>
+      <c r="R3" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="170"/>
-      <c r="T3" s="170"/>
-      <c r="U3" s="170"/>
-      <c r="V3" s="170"/>
-      <c r="W3" s="170" t="s">
+      <c r="S3" s="171"/>
+      <c r="T3" s="171"/>
+      <c r="U3" s="171"/>
+      <c r="V3" s="171"/>
+      <c r="W3" s="171" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="170"/>
-      <c r="Y3" s="170"/>
-      <c r="Z3" s="170"/>
-      <c r="AA3" s="175"/>
+      <c r="X3" s="171"/>
+      <c r="Y3" s="171"/>
+      <c r="Z3" s="171"/>
+      <c r="AA3" s="176"/>
       <c r="AB3"/>
     </row>
     <row r="4" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="161"/>
-      <c r="B4" s="162"/>
-      <c r="C4" s="164"/>
+      <c r="A4" s="162"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="165"/>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
@@ -3782,8 +3779,8 @@
       <c r="AA51" s="73"/>
     </row>
     <row r="52" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="157"/>
-      <c r="B52" s="158"/>
+      <c r="A52" s="158"/>
+      <c r="B52" s="159"/>
       <c r="C52" s="74" t="s">
         <v>81</v>
       </c>
@@ -3803,26 +3800,26 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H52" s="155"/>
-      <c r="I52" s="155"/>
-      <c r="J52" s="155"/>
-      <c r="K52" s="155"/>
-      <c r="L52" s="155"/>
-      <c r="M52" s="155"/>
-      <c r="N52" s="155"/>
-      <c r="O52" s="155"/>
-      <c r="P52" s="155"/>
-      <c r="Q52" s="155"/>
-      <c r="R52" s="155"/>
-      <c r="S52" s="155"/>
-      <c r="T52" s="155"/>
-      <c r="U52" s="155"/>
-      <c r="V52" s="155"/>
-      <c r="W52" s="155"/>
-      <c r="X52" s="155"/>
-      <c r="Y52" s="155"/>
-      <c r="Z52" s="155"/>
-      <c r="AA52" s="156"/>
+      <c r="H52" s="156"/>
+      <c r="I52" s="156"/>
+      <c r="J52" s="156"/>
+      <c r="K52" s="156"/>
+      <c r="L52" s="156"/>
+      <c r="M52" s="156"/>
+      <c r="N52" s="156"/>
+      <c r="O52" s="156"/>
+      <c r="P52" s="156"/>
+      <c r="Q52" s="156"/>
+      <c r="R52" s="156"/>
+      <c r="S52" s="156"/>
+      <c r="T52" s="156"/>
+      <c r="U52" s="156"/>
+      <c r="V52" s="156"/>
+      <c r="W52" s="156"/>
+      <c r="X52" s="156"/>
+      <c r="Y52" s="156"/>
+      <c r="Z52" s="156"/>
+      <c r="AA52" s="157"/>
     </row>
     <row r="53" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="1048576" spans="16:16" x14ac:dyDescent="0.35">
@@ -3871,115 +3868,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="166" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="166"/>
-      <c r="S1" s="166"/>
-      <c r="T1" s="166"/>
-      <c r="U1" s="166"/>
-      <c r="V1" s="166"/>
-      <c r="W1" s="166"/>
-      <c r="X1" s="166"/>
-      <c r="Y1" s="166"/>
-      <c r="Z1" s="166"/>
-      <c r="AA1" s="167"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
+      <c r="P1" s="167"/>
+      <c r="Q1" s="167"/>
+      <c r="R1" s="167"/>
+      <c r="S1" s="167"/>
+      <c r="T1" s="167"/>
+      <c r="U1" s="167"/>
+      <c r="V1" s="167"/>
+      <c r="W1" s="167"/>
+      <c r="X1" s="167"/>
+      <c r="Y1" s="167"/>
+      <c r="Z1" s="167"/>
+      <c r="AA1" s="168"/>
     </row>
     <row r="2" spans="1:32" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="160"/>
-      <c r="C2" s="163" t="s">
+      <c r="B2" s="161"/>
+      <c r="C2" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="168" t="s">
+      <c r="D2" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="168"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="172" t="s">
+      <c r="E2" s="169"/>
+      <c r="F2" s="169"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="173" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="168"/>
-      <c r="J2" s="168"/>
-      <c r="K2" s="168"/>
-      <c r="L2" s="168"/>
-      <c r="M2" s="168"/>
-      <c r="N2" s="168"/>
-      <c r="O2" s="168"/>
-      <c r="P2" s="168"/>
-      <c r="Q2" s="168"/>
-      <c r="R2" s="168"/>
-      <c r="S2" s="168"/>
-      <c r="T2" s="168"/>
-      <c r="U2" s="168"/>
-      <c r="V2" s="168"/>
-      <c r="W2" s="168"/>
-      <c r="X2" s="168"/>
-      <c r="Y2" s="168"/>
-      <c r="Z2" s="168"/>
-      <c r="AA2" s="173"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="169"/>
+      <c r="K2" s="169"/>
+      <c r="L2" s="169"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
+      <c r="O2" s="169"/>
+      <c r="P2" s="169"/>
+      <c r="Q2" s="169"/>
+      <c r="R2" s="169"/>
+      <c r="S2" s="169"/>
+      <c r="T2" s="169"/>
+      <c r="U2" s="169"/>
+      <c r="V2" s="169"/>
+      <c r="W2" s="169"/>
+      <c r="X2" s="169"/>
+      <c r="Y2" s="169"/>
+      <c r="Z2" s="169"/>
+      <c r="AA2" s="174"/>
     </row>
     <row r="3" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="161"/>
-      <c r="B3" s="162"/>
-      <c r="C3" s="164"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="174" t="s">
+      <c r="A3" s="162"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="171"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="171"/>
+      <c r="G3" s="172"/>
+      <c r="H3" s="175" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="170"/>
-      <c r="J3" s="170"/>
-      <c r="K3" s="170"/>
-      <c r="L3" s="170"/>
-      <c r="M3" s="170" t="s">
+      <c r="I3" s="171"/>
+      <c r="J3" s="171"/>
+      <c r="K3" s="171"/>
+      <c r="L3" s="171"/>
+      <c r="M3" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="170"/>
-      <c r="O3" s="170"/>
-      <c r="P3" s="170"/>
-      <c r="Q3" s="170"/>
-      <c r="R3" s="170" t="s">
+      <c r="N3" s="171"/>
+      <c r="O3" s="171"/>
+      <c r="P3" s="171"/>
+      <c r="Q3" s="171"/>
+      <c r="R3" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="170"/>
-      <c r="T3" s="170"/>
-      <c r="U3" s="170"/>
-      <c r="V3" s="170"/>
-      <c r="W3" s="170" t="s">
+      <c r="S3" s="171"/>
+      <c r="T3" s="171"/>
+      <c r="U3" s="171"/>
+      <c r="V3" s="171"/>
+      <c r="W3" s="171" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="170"/>
-      <c r="Y3" s="170"/>
-      <c r="Z3" s="170"/>
-      <c r="AA3" s="175"/>
+      <c r="X3" s="171"/>
+      <c r="Y3" s="171"/>
+      <c r="Z3" s="171"/>
+      <c r="AA3" s="176"/>
       <c r="AB3"/>
     </row>
     <row r="4" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="161"/>
-      <c r="B4" s="162"/>
-      <c r="C4" s="164"/>
+      <c r="A4" s="162"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="165"/>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
@@ -5992,8 +5989,8 @@
       <c r="AA51" s="73"/>
     </row>
     <row r="52" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="157"/>
-      <c r="B52" s="158"/>
+      <c r="A52" s="158"/>
+      <c r="B52" s="159"/>
       <c r="C52" s="74" t="s">
         <v>81</v>
       </c>
@@ -6013,26 +6010,26 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H52" s="155"/>
-      <c r="I52" s="155"/>
-      <c r="J52" s="155"/>
-      <c r="K52" s="155"/>
-      <c r="L52" s="155"/>
-      <c r="M52" s="155"/>
-      <c r="N52" s="155"/>
-      <c r="O52" s="155"/>
-      <c r="P52" s="155"/>
-      <c r="Q52" s="155"/>
-      <c r="R52" s="155"/>
-      <c r="S52" s="155"/>
-      <c r="T52" s="155"/>
-      <c r="U52" s="155"/>
-      <c r="V52" s="155"/>
-      <c r="W52" s="155"/>
-      <c r="X52" s="155"/>
-      <c r="Y52" s="155"/>
-      <c r="Z52" s="155"/>
-      <c r="AA52" s="156"/>
+      <c r="H52" s="156"/>
+      <c r="I52" s="156"/>
+      <c r="J52" s="156"/>
+      <c r="K52" s="156"/>
+      <c r="L52" s="156"/>
+      <c r="M52" s="156"/>
+      <c r="N52" s="156"/>
+      <c r="O52" s="156"/>
+      <c r="P52" s="156"/>
+      <c r="Q52" s="156"/>
+      <c r="R52" s="156"/>
+      <c r="S52" s="156"/>
+      <c r="T52" s="156"/>
+      <c r="U52" s="156"/>
+      <c r="V52" s="156"/>
+      <c r="W52" s="156"/>
+      <c r="X52" s="156"/>
+      <c r="Y52" s="156"/>
+      <c r="Z52" s="156"/>
+      <c r="AA52" s="157"/>
     </row>
     <row r="53" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="1048576" spans="16:16" x14ac:dyDescent="0.35">
@@ -6081,115 +6078,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="166" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="166"/>
-      <c r="S1" s="166"/>
-      <c r="T1" s="166"/>
-      <c r="U1" s="166"/>
-      <c r="V1" s="166"/>
-      <c r="W1" s="166"/>
-      <c r="X1" s="166"/>
-      <c r="Y1" s="166"/>
-      <c r="Z1" s="166"/>
-      <c r="AA1" s="167"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
+      <c r="P1" s="167"/>
+      <c r="Q1" s="167"/>
+      <c r="R1" s="167"/>
+      <c r="S1" s="167"/>
+      <c r="T1" s="167"/>
+      <c r="U1" s="167"/>
+      <c r="V1" s="167"/>
+      <c r="W1" s="167"/>
+      <c r="X1" s="167"/>
+      <c r="Y1" s="167"/>
+      <c r="Z1" s="167"/>
+      <c r="AA1" s="168"/>
     </row>
     <row r="2" spans="1:32" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="160"/>
-      <c r="C2" s="163" t="s">
+      <c r="B2" s="161"/>
+      <c r="C2" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="168" t="s">
+      <c r="D2" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="168"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="172" t="s">
+      <c r="E2" s="169"/>
+      <c r="F2" s="169"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="173" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="168"/>
-      <c r="J2" s="168"/>
-      <c r="K2" s="168"/>
-      <c r="L2" s="168"/>
-      <c r="M2" s="168"/>
-      <c r="N2" s="168"/>
-      <c r="O2" s="168"/>
-      <c r="P2" s="168"/>
-      <c r="Q2" s="168"/>
-      <c r="R2" s="168"/>
-      <c r="S2" s="168"/>
-      <c r="T2" s="168"/>
-      <c r="U2" s="168"/>
-      <c r="V2" s="168"/>
-      <c r="W2" s="168"/>
-      <c r="X2" s="168"/>
-      <c r="Y2" s="168"/>
-      <c r="Z2" s="168"/>
-      <c r="AA2" s="173"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="169"/>
+      <c r="K2" s="169"/>
+      <c r="L2" s="169"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
+      <c r="O2" s="169"/>
+      <c r="P2" s="169"/>
+      <c r="Q2" s="169"/>
+      <c r="R2" s="169"/>
+      <c r="S2" s="169"/>
+      <c r="T2" s="169"/>
+      <c r="U2" s="169"/>
+      <c r="V2" s="169"/>
+      <c r="W2" s="169"/>
+      <c r="X2" s="169"/>
+      <c r="Y2" s="169"/>
+      <c r="Z2" s="169"/>
+      <c r="AA2" s="174"/>
     </row>
     <row r="3" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="161"/>
-      <c r="B3" s="162"/>
-      <c r="C3" s="164"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="174" t="s">
+      <c r="A3" s="162"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="171"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="171"/>
+      <c r="G3" s="172"/>
+      <c r="H3" s="175" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="170"/>
-      <c r="J3" s="170"/>
-      <c r="K3" s="170"/>
-      <c r="L3" s="170"/>
-      <c r="M3" s="170" t="s">
+      <c r="I3" s="171"/>
+      <c r="J3" s="171"/>
+      <c r="K3" s="171"/>
+      <c r="L3" s="171"/>
+      <c r="M3" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="170"/>
-      <c r="O3" s="170"/>
-      <c r="P3" s="170"/>
-      <c r="Q3" s="170"/>
-      <c r="R3" s="170" t="s">
+      <c r="N3" s="171"/>
+      <c r="O3" s="171"/>
+      <c r="P3" s="171"/>
+      <c r="Q3" s="171"/>
+      <c r="R3" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="170"/>
-      <c r="T3" s="170"/>
-      <c r="U3" s="170"/>
-      <c r="V3" s="170"/>
-      <c r="W3" s="170" t="s">
+      <c r="S3" s="171"/>
+      <c r="T3" s="171"/>
+      <c r="U3" s="171"/>
+      <c r="V3" s="171"/>
+      <c r="W3" s="171" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="170"/>
-      <c r="Y3" s="170"/>
-      <c r="Z3" s="170"/>
-      <c r="AA3" s="175"/>
+      <c r="X3" s="171"/>
+      <c r="Y3" s="171"/>
+      <c r="Z3" s="171"/>
+      <c r="AA3" s="176"/>
       <c r="AB3"/>
     </row>
     <row r="4" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="161"/>
-      <c r="B4" s="162"/>
-      <c r="C4" s="164"/>
+      <c r="A4" s="162"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="165"/>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
@@ -6366,10 +6363,10 @@
       <c r="C7" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="177" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="177" t="s">
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="1"/>
@@ -8202,8 +8199,8 @@
       <c r="AA51" s="73"/>
     </row>
     <row r="52" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="157"/>
-      <c r="B52" s="158"/>
+      <c r="A52" s="158"/>
+      <c r="B52" s="159"/>
       <c r="C52" s="74" t="s">
         <v>81</v>
       </c>
@@ -8223,26 +8220,26 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H52" s="155"/>
-      <c r="I52" s="155"/>
-      <c r="J52" s="155"/>
-      <c r="K52" s="155"/>
-      <c r="L52" s="155"/>
-      <c r="M52" s="155"/>
-      <c r="N52" s="155"/>
-      <c r="O52" s="155"/>
-      <c r="P52" s="155"/>
-      <c r="Q52" s="155"/>
-      <c r="R52" s="155"/>
-      <c r="S52" s="155"/>
-      <c r="T52" s="155"/>
-      <c r="U52" s="155"/>
-      <c r="V52" s="155"/>
-      <c r="W52" s="155"/>
-      <c r="X52" s="155"/>
-      <c r="Y52" s="155"/>
-      <c r="Z52" s="155"/>
-      <c r="AA52" s="156"/>
+      <c r="H52" s="156"/>
+      <c r="I52" s="156"/>
+      <c r="J52" s="156"/>
+      <c r="K52" s="156"/>
+      <c r="L52" s="156"/>
+      <c r="M52" s="156"/>
+      <c r="N52" s="156"/>
+      <c r="O52" s="156"/>
+      <c r="P52" s="156"/>
+      <c r="Q52" s="156"/>
+      <c r="R52" s="156"/>
+      <c r="S52" s="156"/>
+      <c r="T52" s="156"/>
+      <c r="U52" s="156"/>
+      <c r="V52" s="156"/>
+      <c r="W52" s="156"/>
+      <c r="X52" s="156"/>
+      <c r="Y52" s="156"/>
+      <c r="Z52" s="156"/>
+      <c r="AA52" s="157"/>
     </row>
     <row r="53" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="1048576" spans="16:16" x14ac:dyDescent="0.35">
@@ -8291,115 +8288,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="166" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="166"/>
-      <c r="S1" s="166"/>
-      <c r="T1" s="166"/>
-      <c r="U1" s="166"/>
-      <c r="V1" s="166"/>
-      <c r="W1" s="166"/>
-      <c r="X1" s="166"/>
-      <c r="Y1" s="166"/>
-      <c r="Z1" s="166"/>
-      <c r="AA1" s="167"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
+      <c r="P1" s="167"/>
+      <c r="Q1" s="167"/>
+      <c r="R1" s="167"/>
+      <c r="S1" s="167"/>
+      <c r="T1" s="167"/>
+      <c r="U1" s="167"/>
+      <c r="V1" s="167"/>
+      <c r="W1" s="167"/>
+      <c r="X1" s="167"/>
+      <c r="Y1" s="167"/>
+      <c r="Z1" s="167"/>
+      <c r="AA1" s="168"/>
     </row>
     <row r="2" spans="1:32" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="160"/>
-      <c r="C2" s="163" t="s">
+      <c r="B2" s="161"/>
+      <c r="C2" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="168" t="s">
+      <c r="D2" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="168"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="172" t="s">
+      <c r="E2" s="169"/>
+      <c r="F2" s="169"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="173" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="168"/>
-      <c r="J2" s="168"/>
-      <c r="K2" s="168"/>
-      <c r="L2" s="168"/>
-      <c r="M2" s="168"/>
-      <c r="N2" s="168"/>
-      <c r="O2" s="168"/>
-      <c r="P2" s="168"/>
-      <c r="Q2" s="168"/>
-      <c r="R2" s="168"/>
-      <c r="S2" s="168"/>
-      <c r="T2" s="168"/>
-      <c r="U2" s="168"/>
-      <c r="V2" s="168"/>
-      <c r="W2" s="168"/>
-      <c r="X2" s="168"/>
-      <c r="Y2" s="168"/>
-      <c r="Z2" s="168"/>
-      <c r="AA2" s="173"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="169"/>
+      <c r="K2" s="169"/>
+      <c r="L2" s="169"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
+      <c r="O2" s="169"/>
+      <c r="P2" s="169"/>
+      <c r="Q2" s="169"/>
+      <c r="R2" s="169"/>
+      <c r="S2" s="169"/>
+      <c r="T2" s="169"/>
+      <c r="U2" s="169"/>
+      <c r="V2" s="169"/>
+      <c r="W2" s="169"/>
+      <c r="X2" s="169"/>
+      <c r="Y2" s="169"/>
+      <c r="Z2" s="169"/>
+      <c r="AA2" s="174"/>
     </row>
     <row r="3" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="161"/>
-      <c r="B3" s="162"/>
-      <c r="C3" s="164"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="174" t="s">
+      <c r="A3" s="162"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="171"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="171"/>
+      <c r="G3" s="172"/>
+      <c r="H3" s="175" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="170"/>
-      <c r="J3" s="170"/>
-      <c r="K3" s="170"/>
-      <c r="L3" s="170"/>
-      <c r="M3" s="170" t="s">
+      <c r="I3" s="171"/>
+      <c r="J3" s="171"/>
+      <c r="K3" s="171"/>
+      <c r="L3" s="171"/>
+      <c r="M3" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="170"/>
-      <c r="O3" s="170"/>
-      <c r="P3" s="170"/>
-      <c r="Q3" s="170"/>
-      <c r="R3" s="170" t="s">
+      <c r="N3" s="171"/>
+      <c r="O3" s="171"/>
+      <c r="P3" s="171"/>
+      <c r="Q3" s="171"/>
+      <c r="R3" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="170"/>
-      <c r="T3" s="170"/>
-      <c r="U3" s="170"/>
-      <c r="V3" s="170"/>
-      <c r="W3" s="170" t="s">
+      <c r="S3" s="171"/>
+      <c r="T3" s="171"/>
+      <c r="U3" s="171"/>
+      <c r="V3" s="171"/>
+      <c r="W3" s="171" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="170"/>
-      <c r="Y3" s="170"/>
-      <c r="Z3" s="170"/>
-      <c r="AA3" s="175"/>
+      <c r="X3" s="171"/>
+      <c r="Y3" s="171"/>
+      <c r="Z3" s="171"/>
+      <c r="AA3" s="176"/>
       <c r="AB3"/>
     </row>
     <row r="4" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="161"/>
-      <c r="B4" s="162"/>
-      <c r="C4" s="164"/>
+      <c r="A4" s="162"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="165"/>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
@@ -8576,10 +8573,10 @@
       <c r="C7" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="177" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="177" t="s">
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="1"/>
@@ -10410,8 +10407,8 @@
       <c r="AA51" s="73"/>
     </row>
     <row r="52" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="157"/>
-      <c r="B52" s="158"/>
+      <c r="A52" s="158"/>
+      <c r="B52" s="159"/>
       <c r="C52" s="74" t="s">
         <v>81</v>
       </c>
@@ -10431,26 +10428,26 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H52" s="155"/>
-      <c r="I52" s="155"/>
-      <c r="J52" s="155"/>
-      <c r="K52" s="155"/>
-      <c r="L52" s="155"/>
-      <c r="M52" s="155"/>
-      <c r="N52" s="155"/>
-      <c r="O52" s="155"/>
-      <c r="P52" s="155"/>
-      <c r="Q52" s="155"/>
-      <c r="R52" s="155"/>
-      <c r="S52" s="155"/>
-      <c r="T52" s="155"/>
-      <c r="U52" s="155"/>
-      <c r="V52" s="155"/>
-      <c r="W52" s="155"/>
-      <c r="X52" s="155"/>
-      <c r="Y52" s="155"/>
-      <c r="Z52" s="155"/>
-      <c r="AA52" s="156"/>
+      <c r="H52" s="156"/>
+      <c r="I52" s="156"/>
+      <c r="J52" s="156"/>
+      <c r="K52" s="156"/>
+      <c r="L52" s="156"/>
+      <c r="M52" s="156"/>
+      <c r="N52" s="156"/>
+      <c r="O52" s="156"/>
+      <c r="P52" s="156"/>
+      <c r="Q52" s="156"/>
+      <c r="R52" s="156"/>
+      <c r="S52" s="156"/>
+      <c r="T52" s="156"/>
+      <c r="U52" s="156"/>
+      <c r="V52" s="156"/>
+      <c r="W52" s="156"/>
+      <c r="X52" s="156"/>
+      <c r="Y52" s="156"/>
+      <c r="Z52" s="156"/>
+      <c r="AA52" s="157"/>
     </row>
     <row r="53" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="1048576" spans="16:16" x14ac:dyDescent="0.35">
@@ -10499,115 +10496,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="166" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="166"/>
-      <c r="S1" s="166"/>
-      <c r="T1" s="166"/>
-      <c r="U1" s="166"/>
-      <c r="V1" s="166"/>
-      <c r="W1" s="166"/>
-      <c r="X1" s="166"/>
-      <c r="Y1" s="166"/>
-      <c r="Z1" s="166"/>
-      <c r="AA1" s="167"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
+      <c r="P1" s="167"/>
+      <c r="Q1" s="167"/>
+      <c r="R1" s="167"/>
+      <c r="S1" s="167"/>
+      <c r="T1" s="167"/>
+      <c r="U1" s="167"/>
+      <c r="V1" s="167"/>
+      <c r="W1" s="167"/>
+      <c r="X1" s="167"/>
+      <c r="Y1" s="167"/>
+      <c r="Z1" s="167"/>
+      <c r="AA1" s="168"/>
     </row>
     <row r="2" spans="1:32" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="160"/>
-      <c r="C2" s="163" t="s">
+      <c r="B2" s="161"/>
+      <c r="C2" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="168" t="s">
+      <c r="D2" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="168"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="172" t="s">
+      <c r="E2" s="169"/>
+      <c r="F2" s="169"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="173" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="168"/>
-      <c r="J2" s="168"/>
-      <c r="K2" s="168"/>
-      <c r="L2" s="168"/>
-      <c r="M2" s="168"/>
-      <c r="N2" s="168"/>
-      <c r="O2" s="168"/>
-      <c r="P2" s="168"/>
-      <c r="Q2" s="168"/>
-      <c r="R2" s="168"/>
-      <c r="S2" s="168"/>
-      <c r="T2" s="168"/>
-      <c r="U2" s="168"/>
-      <c r="V2" s="168"/>
-      <c r="W2" s="168"/>
-      <c r="X2" s="168"/>
-      <c r="Y2" s="168"/>
-      <c r="Z2" s="168"/>
-      <c r="AA2" s="173"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="169"/>
+      <c r="K2" s="169"/>
+      <c r="L2" s="169"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
+      <c r="O2" s="169"/>
+      <c r="P2" s="169"/>
+      <c r="Q2" s="169"/>
+      <c r="R2" s="169"/>
+      <c r="S2" s="169"/>
+      <c r="T2" s="169"/>
+      <c r="U2" s="169"/>
+      <c r="V2" s="169"/>
+      <c r="W2" s="169"/>
+      <c r="X2" s="169"/>
+      <c r="Y2" s="169"/>
+      <c r="Z2" s="169"/>
+      <c r="AA2" s="174"/>
     </row>
     <row r="3" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="161"/>
-      <c r="B3" s="162"/>
-      <c r="C3" s="164"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="174" t="s">
+      <c r="A3" s="162"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="171"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="171"/>
+      <c r="G3" s="172"/>
+      <c r="H3" s="175" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="170"/>
-      <c r="J3" s="170"/>
-      <c r="K3" s="170"/>
-      <c r="L3" s="170"/>
-      <c r="M3" s="170" t="s">
+      <c r="I3" s="171"/>
+      <c r="J3" s="171"/>
+      <c r="K3" s="171"/>
+      <c r="L3" s="171"/>
+      <c r="M3" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="170"/>
-      <c r="O3" s="170"/>
-      <c r="P3" s="170"/>
-      <c r="Q3" s="170"/>
-      <c r="R3" s="170" t="s">
+      <c r="N3" s="171"/>
+      <c r="O3" s="171"/>
+      <c r="P3" s="171"/>
+      <c r="Q3" s="171"/>
+      <c r="R3" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="170"/>
-      <c r="T3" s="170"/>
-      <c r="U3" s="170"/>
-      <c r="V3" s="170"/>
-      <c r="W3" s="170" t="s">
+      <c r="S3" s="171"/>
+      <c r="T3" s="171"/>
+      <c r="U3" s="171"/>
+      <c r="V3" s="171"/>
+      <c r="W3" s="171" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="170"/>
-      <c r="Y3" s="170"/>
-      <c r="Z3" s="170"/>
-      <c r="AA3" s="175"/>
+      <c r="X3" s="171"/>
+      <c r="Y3" s="171"/>
+      <c r="Z3" s="171"/>
+      <c r="AA3" s="176"/>
       <c r="AB3"/>
     </row>
     <row r="4" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="161"/>
-      <c r="B4" s="162"/>
-      <c r="C4" s="164"/>
+      <c r="A4" s="162"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="165"/>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
@@ -10784,10 +10781,10 @@
       <c r="C7" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="177" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="177" t="s">
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="1"/>
@@ -12630,8 +12627,8 @@
       <c r="AA51" s="73"/>
     </row>
     <row r="52" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="157"/>
-      <c r="B52" s="158"/>
+      <c r="A52" s="158"/>
+      <c r="B52" s="159"/>
       <c r="C52" s="74" t="s">
         <v>81</v>
       </c>
@@ -12651,26 +12648,26 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H52" s="155"/>
-      <c r="I52" s="155"/>
-      <c r="J52" s="155"/>
-      <c r="K52" s="155"/>
-      <c r="L52" s="155"/>
-      <c r="M52" s="155"/>
-      <c r="N52" s="155"/>
-      <c r="O52" s="155"/>
-      <c r="P52" s="155"/>
-      <c r="Q52" s="155"/>
-      <c r="R52" s="155"/>
-      <c r="S52" s="155"/>
-      <c r="T52" s="155"/>
-      <c r="U52" s="155"/>
-      <c r="V52" s="155"/>
-      <c r="W52" s="155"/>
-      <c r="X52" s="155"/>
-      <c r="Y52" s="155"/>
-      <c r="Z52" s="155"/>
-      <c r="AA52" s="156"/>
+      <c r="H52" s="156"/>
+      <c r="I52" s="156"/>
+      <c r="J52" s="156"/>
+      <c r="K52" s="156"/>
+      <c r="L52" s="156"/>
+      <c r="M52" s="156"/>
+      <c r="N52" s="156"/>
+      <c r="O52" s="156"/>
+      <c r="P52" s="156"/>
+      <c r="Q52" s="156"/>
+      <c r="R52" s="156"/>
+      <c r="S52" s="156"/>
+      <c r="T52" s="156"/>
+      <c r="U52" s="156"/>
+      <c r="V52" s="156"/>
+      <c r="W52" s="156"/>
+      <c r="X52" s="156"/>
+      <c r="Y52" s="156"/>
+      <c r="Z52" s="156"/>
+      <c r="AA52" s="157"/>
     </row>
     <row r="53" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="1048576" spans="16:16" x14ac:dyDescent="0.35">
@@ -12701,8 +12698,8 @@
   </sheetPr>
   <dimension ref="A1:AF1048576"/>
   <sheetViews>
-    <sheetView zoomScale="116" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E7" sqref="D7:E7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12712,122 +12709,121 @@
     <col min="3" max="3" width="37.6328125" style="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="17" width="2.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="26" width="2.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="27" width="3.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="19.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="29" max="16384" width="10.90625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="26" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="166" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="166"/>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="166"/>
-      <c r="S1" s="166"/>
-      <c r="T1" s="166"/>
-      <c r="U1" s="166"/>
-      <c r="V1" s="166"/>
-      <c r="W1" s="166"/>
-      <c r="X1" s="166"/>
-      <c r="Y1" s="166"/>
-      <c r="Z1" s="166"/>
-      <c r="AA1" s="167"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
+      <c r="P1" s="167"/>
+      <c r="Q1" s="167"/>
+      <c r="R1" s="167"/>
+      <c r="S1" s="167"/>
+      <c r="T1" s="167"/>
+      <c r="U1" s="167"/>
+      <c r="V1" s="167"/>
+      <c r="W1" s="167"/>
+      <c r="X1" s="167"/>
+      <c r="Y1" s="167"/>
+      <c r="Z1" s="167"/>
+      <c r="AA1" s="168"/>
     </row>
     <row r="2" spans="1:32" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="159" t="s">
+      <c r="A2" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="160"/>
-      <c r="C2" s="163" t="s">
+      <c r="B2" s="161"/>
+      <c r="C2" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="168" t="s">
+      <c r="D2" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="168"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="172" t="s">
+      <c r="E2" s="169"/>
+      <c r="F2" s="169"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="173" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="168"/>
-      <c r="J2" s="168"/>
-      <c r="K2" s="168"/>
-      <c r="L2" s="168"/>
-      <c r="M2" s="168"/>
-      <c r="N2" s="168"/>
-      <c r="O2" s="168"/>
-      <c r="P2" s="168"/>
-      <c r="Q2" s="168"/>
-      <c r="R2" s="168"/>
-      <c r="S2" s="168"/>
-      <c r="T2" s="168"/>
-      <c r="U2" s="168"/>
-      <c r="V2" s="168"/>
-      <c r="W2" s="168"/>
-      <c r="X2" s="168"/>
-      <c r="Y2" s="168"/>
-      <c r="Z2" s="168"/>
-      <c r="AA2" s="173"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="169"/>
+      <c r="K2" s="169"/>
+      <c r="L2" s="169"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
+      <c r="O2" s="169"/>
+      <c r="P2" s="169"/>
+      <c r="Q2" s="169"/>
+      <c r="R2" s="169"/>
+      <c r="S2" s="169"/>
+      <c r="T2" s="169"/>
+      <c r="U2" s="169"/>
+      <c r="V2" s="169"/>
+      <c r="W2" s="169"/>
+      <c r="X2" s="169"/>
+      <c r="Y2" s="169"/>
+      <c r="Z2" s="169"/>
+      <c r="AA2" s="174"/>
     </row>
     <row r="3" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="161"/>
-      <c r="B3" s="162"/>
-      <c r="C3" s="164"/>
-      <c r="D3" s="170"/>
-      <c r="E3" s="170"/>
-      <c r="F3" s="170"/>
-      <c r="G3" s="171"/>
-      <c r="H3" s="174" t="s">
+      <c r="A3" s="162"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="171"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="171"/>
+      <c r="G3" s="172"/>
+      <c r="H3" s="175" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="170"/>
-      <c r="J3" s="170"/>
-      <c r="K3" s="170"/>
-      <c r="L3" s="170"/>
-      <c r="M3" s="170" t="s">
+      <c r="I3" s="171"/>
+      <c r="J3" s="171"/>
+      <c r="K3" s="171"/>
+      <c r="L3" s="171"/>
+      <c r="M3" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="170"/>
-      <c r="O3" s="170"/>
-      <c r="P3" s="170"/>
-      <c r="Q3" s="170"/>
-      <c r="R3" s="170" t="s">
+      <c r="N3" s="171"/>
+      <c r="O3" s="171"/>
+      <c r="P3" s="171"/>
+      <c r="Q3" s="171"/>
+      <c r="R3" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="170"/>
-      <c r="T3" s="170"/>
-      <c r="U3" s="170"/>
-      <c r="V3" s="170"/>
-      <c r="W3" s="170" t="s">
+      <c r="S3" s="171"/>
+      <c r="T3" s="171"/>
+      <c r="U3" s="171"/>
+      <c r="V3" s="171"/>
+      <c r="W3" s="171" t="s">
         <v>6</v>
       </c>
-      <c r="X3" s="170"/>
-      <c r="Y3" s="170"/>
-      <c r="Z3" s="170"/>
-      <c r="AA3" s="175"/>
+      <c r="X3" s="171"/>
+      <c r="Y3" s="171"/>
+      <c r="Z3" s="171"/>
+      <c r="AA3" s="176"/>
       <c r="AB3"/>
     </row>
     <row r="4" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="161"/>
-      <c r="B4" s="162"/>
-      <c r="C4" s="164"/>
+      <c r="A4" s="162"/>
+      <c r="B4" s="163"/>
+      <c r="C4" s="165"/>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
@@ -13004,10 +13000,10 @@
       <c r="C7" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="177" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="177" t="s">
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="1"/>
@@ -14107,7 +14103,7 @@
       </c>
       <c r="S33" s="103"/>
       <c r="T33" s="103"/>
-      <c r="U33" s="176" t="s">
+      <c r="U33" s="155" t="s">
         <v>8</v>
       </c>
       <c r="V33" s="27"/>
@@ -14856,8 +14852,8 @@
       <c r="AA51" s="73"/>
     </row>
     <row r="52" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="157"/>
-      <c r="B52" s="158"/>
+      <c r="A52" s="158"/>
+      <c r="B52" s="159"/>
       <c r="C52" s="74" t="s">
         <v>81</v>
       </c>
@@ -14877,26 +14873,26 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H52" s="155"/>
-      <c r="I52" s="155"/>
-      <c r="J52" s="155"/>
-      <c r="K52" s="155"/>
-      <c r="L52" s="155"/>
-      <c r="M52" s="155"/>
-      <c r="N52" s="155"/>
-      <c r="O52" s="155"/>
-      <c r="P52" s="155"/>
-      <c r="Q52" s="155"/>
-      <c r="R52" s="155"/>
-      <c r="S52" s="155"/>
-      <c r="T52" s="155"/>
-      <c r="U52" s="155"/>
-      <c r="V52" s="155"/>
-      <c r="W52" s="155"/>
-      <c r="X52" s="155"/>
-      <c r="Y52" s="155"/>
-      <c r="Z52" s="155"/>
-      <c r="AA52" s="156"/>
+      <c r="H52" s="156"/>
+      <c r="I52" s="156"/>
+      <c r="J52" s="156"/>
+      <c r="K52" s="156"/>
+      <c r="L52" s="156"/>
+      <c r="M52" s="156"/>
+      <c r="N52" s="156"/>
+      <c r="O52" s="156"/>
+      <c r="P52" s="156"/>
+      <c r="Q52" s="156"/>
+      <c r="R52" s="156"/>
+      <c r="S52" s="156"/>
+      <c r="T52" s="156"/>
+      <c r="U52" s="156"/>
+      <c r="V52" s="156"/>
+      <c r="W52" s="156"/>
+      <c r="X52" s="156"/>
+      <c r="Y52" s="156"/>
+      <c r="Z52" s="156"/>
+      <c r="AA52" s="157"/>
     </row>
     <row r="53" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="1048576" spans="16:16" x14ac:dyDescent="0.35">

</xml_diff>